<commit_message>
database restructure, closes #5
</commit_message>
<xml_diff>
--- a/inst/app/camera_trap_templates.xlsx
+++ b/inst/app/camera_trap_templates.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="197">
   <si>
     <t xml:space="preserve">SiteID</t>
   </si>
@@ -86,7 +86,7 @@
     <t xml:space="preserve">01:32:47</t>
   </si>
   <si>
-    <t xml:space="preserve">/Library/Frameworks/R.framework/Versions/4.1/Resources/library/weda/dummydata/images/2602</t>
+    <t xml:space="preserve">/Users/justincally/Documents/Work/R Repositories/weda/inst/dummydata/images/2602</t>
   </si>
   <si>
     <t xml:space="preserve">2602__2021-10-17__01-32-47(5).JPG</t>
@@ -107,7 +107,7 @@
     <t xml:space="preserve">18:15:26</t>
   </si>
   <si>
-    <t xml:space="preserve">/Library/Frameworks/R.framework/Versions/4.1/Resources/library/weda/dummydata/images/43134</t>
+    <t xml:space="preserve">/Users/justincally/Documents/Work/R Repositories/weda/inst/dummydata/images/43134</t>
   </si>
   <si>
     <t xml:space="preserve">43134__2021-11-16__18-15-26(22).JPG</t>
@@ -134,7 +134,7 @@
     <t xml:space="preserve">08:50:17</t>
   </si>
   <si>
-    <t xml:space="preserve">/Library/Frameworks/R.framework/Versions/4.1/Resources/library/weda/dummydata/images/56505/A</t>
+    <t xml:space="preserve">/Users/justincally/Documents/Work/R Repositories/weda/inst/dummydata/images/56505/A</t>
   </si>
   <si>
     <t xml:space="preserve">56505__2021-11-30__08-50-17(2).JPG</t>
@@ -155,7 +155,7 @@
     <t xml:space="preserve">08:50:57</t>
   </si>
   <si>
-    <t xml:space="preserve">/Library/Frameworks/R.framework/Versions/4.1/Resources/library/weda/dummydata/images/56505/B</t>
+    <t xml:space="preserve">/Users/justincally/Documents/Work/R Repositories/weda/inst/dummydata/images/56505/B</t>
   </si>
   <si>
     <t xml:space="preserve">56505__2021-11-30__08-50-57(59).JPG</t>
@@ -176,7 +176,7 @@
     <t xml:space="preserve">14:30:38</t>
   </si>
   <si>
-    <t xml:space="preserve">/Library/Frameworks/R.framework/Versions/4.1/Resources/library/weda/dummydata/images/832</t>
+    <t xml:space="preserve">/Users/justincally/Documents/Work/R Repositories/weda/inst/dummydata/images/832</t>
   </si>
   <si>
     <t xml:space="preserve">832__2021-10-21__14-30-38(8).JPG</t>
@@ -191,7 +191,7 @@
     <t xml:space="preserve">18:09:19</t>
   </si>
   <si>
-    <t xml:space="preserve">/Library/Frameworks/R.framework/Versions/4.1/Resources/library/weda/dummydata/images/9941</t>
+    <t xml:space="preserve">/Users/justincally/Documents/Work/R Repositories/weda/inst/dummydata/images/9941</t>
   </si>
   <si>
     <t xml:space="preserve">9941__2021-10-14__18-09-19(13).JPG</t>
@@ -248,6 +248,12 @@
     <t xml:space="preserve">CameraHeight</t>
   </si>
   <si>
+    <t xml:space="preserve">CameraBearing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CameraSlope</t>
+  </si>
+  <si>
     <t xml:space="preserve">CameraID</t>
   </si>
   <si>
@@ -263,6 +269,18 @@
     <t xml:space="preserve">CameraPhotosPerTrigger</t>
   </si>
   <si>
+    <t xml:space="preserve">CameraQuietPeriod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BaitedUnbaited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BaitType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BaitDistance</t>
+  </si>
+  <si>
     <t xml:space="preserve">14:18:00</t>
   </si>
   <si>
@@ -281,6 +299,12 @@
     <t xml:space="preserve">Rapidfire</t>
   </si>
   <si>
+    <t xml:space="preserve">Unbaited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
     <t xml:space="preserve">10:56:00</t>
   </si>
   <si>
@@ -332,25 +356,28 @@
     <t xml:space="preserve">AllSpeciesTagged</t>
   </si>
   <si>
-    <t xml:space="preserve">BaitedUnbaited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BaitType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monitoring deer distribution, abundance, and impacts across Victoria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StatewideDeer</t>
+    <t xml:space="preserve">DistanceForAllSpecies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProjectDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProjectLeader</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dummy Data Project 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DummyData</t>
   </si>
   <si>
     <t xml:space="preserve">Terrestrial</t>
   </si>
   <si>
-    <t xml:space="preserve">Unbaited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">None</t>
+    <t xml:space="preserve">Dummy Data for the tutorial on uploading data to the database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Justin Cally</t>
   </si>
   <si>
     <t xml:space="preserve">schema</t>
@@ -1459,6 +1486,24 @@
       <c r="S1" t="s">
         <v>81</v>
       </c>
+      <c r="T1" t="s">
+        <v>82</v>
+      </c>
+      <c r="U1" t="s">
+        <v>83</v>
+      </c>
+      <c r="V1" t="s">
+        <v>84</v>
+      </c>
+      <c r="W1" t="s">
+        <v>85</v>
+      </c>
+      <c r="X1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -1478,13 +1523,13 @@
         <v>44483</v>
       </c>
       <c r="G2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>44537</v>
       </c>
       <c r="I2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1497,21 +1542,37 @@
       <c r="N2" t="n">
         <v>1</v>
       </c>
-      <c r="O2" t="s">
-        <v>84</v>
-      </c>
-      <c r="P2" t="s">
-        <v>85</v>
+      <c r="O2" t="n">
+        <v>180</v>
+      </c>
+      <c r="P2" t="n">
+        <v>2</v>
       </c>
       <c r="Q2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="R2" t="s">
-        <v>87</v>
-      </c>
-      <c r="S2" t="n">
+        <v>91</v>
+      </c>
+      <c r="S2" t="s">
+        <v>92</v>
+      </c>
+      <c r="T2" t="s">
+        <v>93</v>
+      </c>
+      <c r="U2" t="n">
         <v>5</v>
       </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="s">
+        <v>94</v>
+      </c>
+      <c r="X2" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -1531,13 +1592,13 @@
         <v>44484</v>
       </c>
       <c r="G3" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>44537</v>
       </c>
       <c r="I3" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>44518.6641319444</v>
@@ -1554,21 +1615,37 @@
       <c r="N3" t="n">
         <v>1</v>
       </c>
-      <c r="O3" t="s">
-        <v>90</v>
-      </c>
-      <c r="P3" t="s">
-        <v>85</v>
+      <c r="O3" t="n">
+        <v>168</v>
+      </c>
+      <c r="P3" t="n">
+        <v>4</v>
       </c>
       <c r="Q3" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="R3" t="s">
-        <v>87</v>
-      </c>
-      <c r="S3" t="n">
+        <v>91</v>
+      </c>
+      <c r="S3" t="s">
+        <v>92</v>
+      </c>
+      <c r="T3" t="s">
+        <v>93</v>
+      </c>
+      <c r="U3" t="n">
         <v>5</v>
       </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="s">
+        <v>94</v>
+      </c>
+      <c r="X3" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -1588,13 +1665,13 @@
         <v>44484</v>
       </c>
       <c r="G4" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>44538</v>
       </c>
       <c r="I4" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1607,21 +1684,37 @@
       <c r="N4" t="n">
         <v>1</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" t="n">
+        <v>175</v>
+      </c>
+      <c r="P4" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>100</v>
+      </c>
+      <c r="R4" t="s">
+        <v>91</v>
+      </c>
+      <c r="S4" t="s">
         <v>92</v>
       </c>
-      <c r="P4" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>86</v>
-      </c>
-      <c r="R4" t="s">
-        <v>87</v>
-      </c>
-      <c r="S4" t="n">
+      <c r="T4" t="s">
+        <v>93</v>
+      </c>
+      <c r="U4" t="n">
         <v>5</v>
       </c>
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" t="s">
+        <v>94</v>
+      </c>
+      <c r="X4" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -1641,13 +1734,13 @@
         <v>44495</v>
       </c>
       <c r="G5" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>44551</v>
       </c>
       <c r="I5" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1660,21 +1753,37 @@
       <c r="N5" t="n">
         <v>1</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" t="n">
+        <v>200</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>103</v>
+      </c>
+      <c r="R5" t="s">
+        <v>91</v>
+      </c>
+      <c r="S5" t="s">
+        <v>92</v>
+      </c>
+      <c r="T5" t="s">
+        <v>93</v>
+      </c>
+      <c r="U5" t="n">
+        <v>5</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" t="s">
+        <v>94</v>
+      </c>
+      <c r="X5" t="s">
         <v>95</v>
       </c>
-      <c r="P5" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>86</v>
-      </c>
-      <c r="R5" t="s">
-        <v>87</v>
-      </c>
-      <c r="S5" t="n">
-        <v>5</v>
-      </c>
+      <c r="Y5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -1696,13 +1805,13 @@
         <v>44495</v>
       </c>
       <c r="G6" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>44546</v>
       </c>
       <c r="I6" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -1715,21 +1824,37 @@
       <c r="N6" t="n">
         <v>1</v>
       </c>
-      <c r="O6" t="s">
-        <v>98</v>
-      </c>
-      <c r="P6" t="s">
-        <v>85</v>
+      <c r="O6" t="n">
+        <v>185</v>
+      </c>
+      <c r="P6" t="n">
+        <v>8</v>
       </c>
       <c r="Q6" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="R6" t="s">
-        <v>87</v>
-      </c>
-      <c r="S6" t="n">
+        <v>91</v>
+      </c>
+      <c r="S6" t="s">
+        <v>92</v>
+      </c>
+      <c r="T6" t="s">
+        <v>93</v>
+      </c>
+      <c r="U6" t="n">
         <v>5</v>
       </c>
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="s">
+        <v>94</v>
+      </c>
+      <c r="X6" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -1751,13 +1876,13 @@
         <v>44495</v>
       </c>
       <c r="G7" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>44546</v>
       </c>
       <c r="I7" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -1770,21 +1895,37 @@
       <c r="N7" t="n">
         <v>1</v>
       </c>
-      <c r="O7" t="s">
-        <v>99</v>
-      </c>
-      <c r="P7" t="s">
-        <v>85</v>
+      <c r="O7" t="n">
+        <v>180</v>
+      </c>
+      <c r="P7" t="n">
+        <v>6</v>
       </c>
       <c r="Q7" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="R7" t="s">
-        <v>87</v>
-      </c>
-      <c r="S7" t="n">
+        <v>91</v>
+      </c>
+      <c r="S7" t="s">
+        <v>92</v>
+      </c>
+      <c r="T7" t="s">
+        <v>93</v>
+      </c>
+      <c r="U7" t="n">
         <v>5</v>
       </c>
+      <c r="V7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" t="s">
+        <v>94</v>
+      </c>
+      <c r="X7" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1802,48 +1943,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C1" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="D1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="E1" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="F1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="G1" t="s">
-        <v>106</v>
+        <v>114</v>
+      </c>
+      <c r="H1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>110</v>
+      <c r="F2" t="b">
+        <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>111</v>
+        <v>119</v>
+      </c>
+      <c r="H2" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1862,348 +2009,348 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B1" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="C1" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="D1" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="E1" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="F1" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="G1" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="H1" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="I1" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="D2" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E2" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="F2" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G2" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="H2"/>
       <c r="I2" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="F3" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G3" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="H3"/>
       <c r="I3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="D4" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="F4" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G4" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="H4"/>
       <c r="I4" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="D5" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="F5" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G5" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="H5"/>
       <c r="I5" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C6" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="D6" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E6" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="F6" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G6" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="H6"/>
       <c r="I6" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="D7" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E7" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="F7" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G7" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="H7"/>
       <c r="I7" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="D8" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E8" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="F8" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G8" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="H8"/>
       <c r="I8" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" t="s">
         <v>134</v>
       </c>
-      <c r="C9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D9" t="s">
-        <v>124</v>
-      </c>
-      <c r="E9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F9" t="s">
-        <v>125</v>
-      </c>
       <c r="G9" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="H9"/>
       <c r="I9" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
         <v>134</v>
       </c>
-      <c r="C10" t="s">
-        <v>135</v>
-      </c>
-      <c r="D10" t="s">
-        <v>124</v>
-      </c>
-      <c r="E10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>125</v>
-      </c>
       <c r="G10" t="s">
+        <v>145</v>
+      </c>
+      <c r="H10" t="s">
+        <v>146</v>
+      </c>
+      <c r="I10" t="s">
         <v>136</v>
-      </c>
-      <c r="H10" t="s">
-        <v>137</v>
-      </c>
-      <c r="I10" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D11" t="s">
+        <v>133</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
         <v>134</v>
       </c>
-      <c r="C11" t="s">
-        <v>135</v>
-      </c>
-      <c r="D11" t="s">
-        <v>124</v>
-      </c>
-      <c r="E11" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
-        <v>125</v>
-      </c>
       <c r="G11" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="H11" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="I11" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D12" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E12" t="s">
         <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="G12" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="H12" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="I12" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B13" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C13" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D13" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E13" t="s">
         <v>4</v>
@@ -2212,612 +2359,612 @@
         <v>4</v>
       </c>
       <c r="G13" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="H13" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="I13" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B14" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C14" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D14" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G14" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="H14" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="I14" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B15" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C15" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D15" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="G15" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="H15"/>
       <c r="I15" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B16" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C16" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D16" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="G16" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="H16"/>
       <c r="I16" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C17" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D17" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="G17" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="H17"/>
       <c r="I17" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B18" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C18" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D18" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
       </c>
       <c r="F18" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="G18" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="H18"/>
       <c r="I18" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B19" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C19" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D19" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G19" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="H19"/>
       <c r="I19" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B20" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C20" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D20" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E20" t="s">
         <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G20" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="H20"/>
       <c r="I20" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B21" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C21" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D21" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E21" t="s">
         <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G21" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="H21"/>
       <c r="I21" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B22" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C22" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D22" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E22" t="s">
         <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G22" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="H22"/>
       <c r="I22" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B23" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C23" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D23" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E23" t="s">
         <v>14</v>
       </c>
       <c r="F23" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="G23" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="H23"/>
       <c r="I23" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B24" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C24" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D24" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E24" t="s">
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G24" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="H24" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="I24" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B25" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C25" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D25" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E25" t="s">
         <v>16</v>
       </c>
       <c r="F25" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G25" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="H25" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="I25" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B26" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C26" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D26" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E26" t="s">
         <v>17</v>
       </c>
       <c r="F26" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="G26" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="H26" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="I26" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B27" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C27" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D27" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E27" t="s">
         <v>18</v>
       </c>
       <c r="F27" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G27" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H27" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="I27" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B28" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C28" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D28" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E28" t="s">
         <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="G28" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="H28"/>
       <c r="I28" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B29" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C29" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D29" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E29" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="F29" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G29" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="H29"/>
       <c r="I29" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B30" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C30" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D30" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E30" t="s">
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G30" t="s">
+        <v>145</v>
+      </c>
+      <c r="H30" t="s">
+        <v>146</v>
+      </c>
+      <c r="I30" t="s">
         <v>136</v>
-      </c>
-      <c r="H30" t="s">
-        <v>137</v>
-      </c>
-      <c r="I30" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B31" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C31" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D31" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E31" t="s">
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G31" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="H31" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="I31" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B32" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C32" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D32" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E32" t="s">
         <v>19</v>
       </c>
       <c r="F32" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="G32" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="H32"/>
       <c r="I32" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B33" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C33" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D33" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E33" t="s">
         <v>66</v>
       </c>
       <c r="F33" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="G33" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="H33" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="I33" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B34" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C34" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D34" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E34" t="s">
         <v>67</v>
       </c>
       <c r="F34" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="G34" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="H34" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="I34" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B35" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C35" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D35" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E35" t="s">
         <v>68</v>
@@ -2826,56 +2973,56 @@
         <v>4</v>
       </c>
       <c r="G35" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="H35" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="I35" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B36" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C36" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D36" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E36" t="s">
         <v>69</v>
       </c>
       <c r="F36" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="G36" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="H36" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="I36" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B37" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C37" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D37" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E37" t="s">
         <v>70</v>
@@ -2884,312 +3031,312 @@
         <v>4</v>
       </c>
       <c r="G37" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="H37" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="I37" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B38" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C38" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D38" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E38" t="s">
         <v>71</v>
       </c>
       <c r="F38" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="G38" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="H38" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="I38" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B39" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C39" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D39" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E39" t="s">
         <v>72</v>
       </c>
       <c r="F39" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="G39" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="H39"/>
       <c r="I39" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B40" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C40" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D40" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E40" t="s">
         <v>73</v>
       </c>
       <c r="F40" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="G40" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="H40"/>
       <c r="I40" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B41" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C41" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D41" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E41" t="s">
         <v>74</v>
       </c>
       <c r="F41" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="G41" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="H41"/>
       <c r="I41" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B42" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C42" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D42" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E42" t="s">
         <v>75</v>
       </c>
       <c r="F42" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="G42" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="H42"/>
       <c r="I42" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B43" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C43" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D43" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E43" t="s">
         <v>76</v>
       </c>
       <c r="F43" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="G43" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="H43"/>
       <c r="I43" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B44" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C44" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D44" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E44" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F44" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G44" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="H44"/>
       <c r="I44" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B45" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C45" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D45" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E45" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F45" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G45" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="H45"/>
       <c r="I45" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B46" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C46" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D46" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E46" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F46" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G46" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="H46"/>
       <c r="I46" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B47" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C47" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D47" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E47" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F47" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G47" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="H47"/>
       <c r="I47" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B48" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C48" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D48" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E48" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F48" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="G48" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="H48"/>
       <c r="I48" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>